<commit_message>
Move to double factor logit instead of weibull + vintaging for sales
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/YBCY/Years Before Current Year.xlsx
+++ b/InputData/plcy-schd/YBCY/Years Before Current Year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\plcy-schd\YBCY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\plcy-schd\YBSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{382695BC-07B5-422C-B751-853533A45C0D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D969254A-CAA9-41E1-8738-B9F4D5E647F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6DBE016C-1CB8-4908-93B0-224380CD752B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6DBE016C-1CB8-4908-93B0-224380CD752B}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working version of stock turnover piece
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/YBCY/Years Before Current Year.xlsx
+++ b/InputData/plcy-schd/YBCY/Years Before Current Year.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\plcy-schd\YBSY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\plcy-schd\YBCY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D969254A-CAA9-41E1-8738-B9F4D5E647F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1965D35-2FD7-4284-9605-DED523ED7AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6DBE016C-1CB8-4908-93B0-224380CD752B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6DBE016C-1CB8-4908-93B0-224380CD752B}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="YBCY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>YBCY Years Before Current Year</t>
   </si>
@@ -125,6 +125,102 @@
   </si>
   <si>
     <t>Year2018</t>
+  </si>
+  <si>
+    <t>Year2019</t>
+  </si>
+  <si>
+    <t>Year2020</t>
+  </si>
+  <si>
+    <t>Year2021</t>
+  </si>
+  <si>
+    <t>Year2022</t>
+  </si>
+  <si>
+    <t>Year2023</t>
+  </si>
+  <si>
+    <t>Year2024</t>
+  </si>
+  <si>
+    <t>Year2025</t>
+  </si>
+  <si>
+    <t>Year2026</t>
+  </si>
+  <si>
+    <t>Year2027</t>
+  </si>
+  <si>
+    <t>Year2028</t>
+  </si>
+  <si>
+    <t>Year2029</t>
+  </si>
+  <si>
+    <t>Year2030</t>
+  </si>
+  <si>
+    <t>Year2031</t>
+  </si>
+  <si>
+    <t>Year2032</t>
+  </si>
+  <si>
+    <t>Year2033</t>
+  </si>
+  <si>
+    <t>Year2034</t>
+  </si>
+  <si>
+    <t>Year2035</t>
+  </si>
+  <si>
+    <t>Year2036</t>
+  </si>
+  <si>
+    <t>Year2037</t>
+  </si>
+  <si>
+    <t>Year2038</t>
+  </si>
+  <si>
+    <t>Year2039</t>
+  </si>
+  <si>
+    <t>Year2040</t>
+  </si>
+  <si>
+    <t>Year2041</t>
+  </si>
+  <si>
+    <t>Year2042</t>
+  </si>
+  <si>
+    <t>Year2043</t>
+  </si>
+  <si>
+    <t>Year2044</t>
+  </si>
+  <si>
+    <t>Year2045</t>
+  </si>
+  <si>
+    <t>Year2046</t>
+  </si>
+  <si>
+    <t>Year2047</t>
+  </si>
+  <si>
+    <t>Year2048</t>
+  </si>
+  <si>
+    <t>Year2049</t>
+  </si>
+  <si>
+    <t>Year2050</t>
   </si>
 </sst>
 </file>
@@ -514,10 +610,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AF62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="E23" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:AF62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,7 +2717,7 @@
         <v>30</v>
       </c>
       <c r="R17">
-        <f t="shared" ref="R17:AF30" si="3">R$1-_xlfn.NUMBERVALUE(RIGHT($A17,4))</f>
+        <f t="shared" ref="R17:AF31" si="3">R$1-_xlfn.NUMBERVALUE(RIGHT($A17,4))</f>
         <v>31</v>
       </c>
       <c r="S17">
@@ -2815,7 +2911,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:Q30" si="4">B$1-_xlfn.NUMBERVALUE(RIGHT($A19,4))</f>
+        <f t="shared" ref="B19:Q34" si="4">B$1-_xlfn.NUMBERVALUE(RIGHT($A19,4))</f>
         <v>13</v>
       </c>
       <c r="C19">
@@ -4356,6 +4452,4134 @@
       <c r="AF30">
         <f t="shared" si="3"/>
         <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:AF40" si="5">C$1-_xlfn.NUMBERVALUE(RIGHT($A32,4))</f>
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:Q62" si="6">B$1-_xlfn.NUMBERVALUE(RIGHT($A35,4))</f>
+        <v>-3</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AE35">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="6"/>
+        <v>-6</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AE38">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="6"/>
+        <v>-7</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AE39">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="6"/>
+        <v>-8</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="5"/>
+        <v>-7</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="5"/>
+        <v>-6</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="5"/>
+        <v>-4</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="6"/>
+        <v>-9</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ref="C41:AF49" si="7">C$1-_xlfn.NUMBERVALUE(RIGHT($A41,4))</f>
+        <v>-8</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="AC41">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="AE41">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="6"/>
+        <v>-10</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="6"/>
+        <v>-11</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AA43">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AB43">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AC43">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AD43">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="AE43">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="AF43">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="6"/>
+        <v>-12</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AC44">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AD44">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AE44">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="AF44">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="6"/>
+        <v>-13</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="7"/>
+        <v>-12</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="AB45">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AC45">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AD45">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AE45">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AF45">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="6"/>
+        <v>-14</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="7"/>
+        <v>-13</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="7"/>
+        <v>-12</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="AC46">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AD46">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AF46">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="6"/>
+        <v>-15</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="7"/>
+        <v>-14</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="7"/>
+        <v>-13</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="7"/>
+        <v>-12</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="AA47">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="AC47">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="AD47">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AE47">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AF47">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="6"/>
+        <v>-16</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="7"/>
+        <v>-15</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="7"/>
+        <v>-14</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="7"/>
+        <v>-13</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="7"/>
+        <v>-12</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AA48">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="AB48">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AC48">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="AD48">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="AE48">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AF48">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="6"/>
+        <v>-17</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="7"/>
+        <v>-16</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="7"/>
+        <v>-15</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="7"/>
+        <v>-14</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="7"/>
+        <v>-13</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="7"/>
+        <v>-12</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="7"/>
+        <v>-11</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="7"/>
+        <v>-10</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="7"/>
+        <v>-9</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="7"/>
+        <v>-8</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="7"/>
+        <v>-7</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="7"/>
+        <v>-6</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="R49">
+        <f t="shared" ref="C49:AF57" si="8">R$1-_xlfn.NUMBERVALUE(RIGHT($A49,4))</f>
+        <v>-1</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="AC49">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="AD49">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="AE49">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="AF49">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="6"/>
+        <v>-18</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AA50">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AB50">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AC50">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="AD50">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="AE50">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="AF50">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="6"/>
+        <v>-19</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AA51">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AB51">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AC51">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AD51">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="AE51">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="AF51">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="6"/>
+        <v>-20</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="Y52">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AA52">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AB52">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AC52">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AE52">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="AF52">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="6"/>
+        <v>-21</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="8"/>
+        <v>-20</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Y53">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="Z53">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="AA53">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AB53">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AC53">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AE53">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AF53">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="6"/>
+        <v>-22</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="8"/>
+        <v>-21</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="8"/>
+        <v>-20</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Z54">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AA54">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="AB54">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AC54">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AD54">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AE54">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AF54">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="6"/>
+        <v>-23</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="8"/>
+        <v>-22</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="8"/>
+        <v>-21</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="8"/>
+        <v>-20</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="X55">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="Y55">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z55">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AA55">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AB55">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="AC55">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AD55">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AE55">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AF55">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="6"/>
+        <v>-24</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="8"/>
+        <v>-23</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="8"/>
+        <v>-22</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="8"/>
+        <v>-21</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="8"/>
+        <v>-20</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="W56">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="X56">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="Y56">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="Z56">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AB56">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AC56">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="AD56">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AE56">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AF56">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="6"/>
+        <v>-25</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="8"/>
+        <v>-24</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="8"/>
+        <v>-23</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="8"/>
+        <v>-22</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="8"/>
+        <v>-21</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="8"/>
+        <v>-20</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="8"/>
+        <v>-19</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="8"/>
+        <v>-18</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="8"/>
+        <v>-17</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="8"/>
+        <v>-16</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="8"/>
+        <v>-15</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="8"/>
+        <v>-14</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="8"/>
+        <v>-13</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="8"/>
+        <v>-12</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="8"/>
+        <v>-11</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="8"/>
+        <v>-10</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="8"/>
+        <v>-9</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="8"/>
+        <v>-8</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="8"/>
+        <v>-7</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="8"/>
+        <v>-6</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="8"/>
+        <v>-5</v>
+      </c>
+      <c r="W57">
+        <f t="shared" si="8"/>
+        <v>-4</v>
+      </c>
+      <c r="X57">
+        <f t="shared" si="8"/>
+        <v>-3</v>
+      </c>
+      <c r="Y57">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="Z57">
+        <f t="shared" si="8"/>
+        <v>-1</v>
+      </c>
+      <c r="AA57">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB57">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="AC57">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="AD57">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="AE57">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AF57">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="6"/>
+        <v>-26</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:AF62" si="9">C$1-_xlfn.NUMBERVALUE(RIGHT($A58,4))</f>
+        <v>-25</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="9"/>
+        <v>-24</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="9"/>
+        <v>-23</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="9"/>
+        <v>-22</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="9"/>
+        <v>-21</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="9"/>
+        <v>-20</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="9"/>
+        <v>-19</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="9"/>
+        <v>-18</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="9"/>
+        <v>-17</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="9"/>
+        <v>-16</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="9"/>
+        <v>-15</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="9"/>
+        <v>-14</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="9"/>
+        <v>-13</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="9"/>
+        <v>-12</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="9"/>
+        <v>-11</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="9"/>
+        <v>-10</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="9"/>
+        <v>-9</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="9"/>
+        <v>-8</v>
+      </c>
+      <c r="U58">
+        <f t="shared" si="9"/>
+        <v>-7</v>
+      </c>
+      <c r="V58">
+        <f t="shared" si="9"/>
+        <v>-6</v>
+      </c>
+      <c r="W58">
+        <f t="shared" si="9"/>
+        <v>-5</v>
+      </c>
+      <c r="X58">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="Y58">
+        <f t="shared" si="9"/>
+        <v>-3</v>
+      </c>
+      <c r="Z58">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="AA58">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="AB58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC58">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AD58">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="AE58">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="AF58">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="6"/>
+        <v>-27</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="9"/>
+        <v>-26</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="9"/>
+        <v>-25</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="9"/>
+        <v>-24</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="9"/>
+        <v>-23</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="9"/>
+        <v>-22</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="9"/>
+        <v>-21</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="9"/>
+        <v>-20</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="9"/>
+        <v>-19</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="9"/>
+        <v>-18</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="9"/>
+        <v>-17</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="9"/>
+        <v>-16</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="9"/>
+        <v>-15</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="9"/>
+        <v>-14</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="9"/>
+        <v>-13</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="9"/>
+        <v>-12</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="9"/>
+        <v>-11</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="9"/>
+        <v>-10</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="9"/>
+        <v>-9</v>
+      </c>
+      <c r="U59">
+        <f t="shared" si="9"/>
+        <v>-8</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="9"/>
+        <v>-7</v>
+      </c>
+      <c r="W59">
+        <f t="shared" si="9"/>
+        <v>-6</v>
+      </c>
+      <c r="X59">
+        <f t="shared" si="9"/>
+        <v>-5</v>
+      </c>
+      <c r="Y59">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="Z59">
+        <f t="shared" si="9"/>
+        <v>-3</v>
+      </c>
+      <c r="AA59">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="AB59">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="AC59">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD59">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AE59">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="AF59">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="6"/>
+        <v>-28</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="9"/>
+        <v>-27</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="9"/>
+        <v>-26</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="9"/>
+        <v>-25</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="9"/>
+        <v>-24</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="9"/>
+        <v>-23</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="9"/>
+        <v>-22</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="9"/>
+        <v>-21</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="9"/>
+        <v>-20</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="9"/>
+        <v>-19</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="9"/>
+        <v>-18</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="9"/>
+        <v>-17</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="9"/>
+        <v>-16</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="9"/>
+        <v>-15</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="9"/>
+        <v>-14</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="9"/>
+        <v>-13</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="9"/>
+        <v>-12</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="9"/>
+        <v>-11</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="9"/>
+        <v>-10</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="9"/>
+        <v>-9</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="9"/>
+        <v>-8</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="9"/>
+        <v>-7</v>
+      </c>
+      <c r="X60">
+        <f t="shared" si="9"/>
+        <v>-6</v>
+      </c>
+      <c r="Y60">
+        <f t="shared" si="9"/>
+        <v>-5</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="9"/>
+        <v>-3</v>
+      </c>
+      <c r="AB60">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="AC60">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="AD60">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AF60">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="6"/>
+        <v>-29</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="9"/>
+        <v>-28</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="9"/>
+        <v>-27</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="9"/>
+        <v>-26</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="9"/>
+        <v>-25</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="9"/>
+        <v>-24</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="9"/>
+        <v>-23</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="9"/>
+        <v>-22</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="9"/>
+        <v>-21</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="9"/>
+        <v>-20</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="9"/>
+        <v>-19</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="9"/>
+        <v>-18</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="9"/>
+        <v>-17</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="9"/>
+        <v>-16</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="9"/>
+        <v>-15</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="9"/>
+        <v>-14</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="9"/>
+        <v>-13</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="9"/>
+        <v>-12</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="9"/>
+        <v>-11</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="9"/>
+        <v>-10</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="9"/>
+        <v>-9</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="9"/>
+        <v>-8</v>
+      </c>
+      <c r="X61">
+        <f t="shared" si="9"/>
+        <v>-7</v>
+      </c>
+      <c r="Y61">
+        <f t="shared" si="9"/>
+        <v>-6</v>
+      </c>
+      <c r="Z61">
+        <f t="shared" si="9"/>
+        <v>-5</v>
+      </c>
+      <c r="AA61">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="AB61">
+        <f t="shared" si="9"/>
+        <v>-3</v>
+      </c>
+      <c r="AC61">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="AD61">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF61">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="6"/>
+        <v>-30</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="9"/>
+        <v>-29</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="9"/>
+        <v>-28</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="9"/>
+        <v>-27</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="9"/>
+        <v>-26</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="9"/>
+        <v>-25</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="9"/>
+        <v>-24</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="9"/>
+        <v>-23</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="9"/>
+        <v>-22</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="9"/>
+        <v>-21</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="9"/>
+        <v>-20</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="9"/>
+        <v>-19</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="9"/>
+        <v>-18</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="9"/>
+        <v>-17</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="9"/>
+        <v>-16</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="9"/>
+        <v>-15</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="9"/>
+        <v>-14</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="9"/>
+        <v>-13</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="9"/>
+        <v>-12</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="9"/>
+        <v>-11</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="9"/>
+        <v>-10</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="9"/>
+        <v>-9</v>
+      </c>
+      <c r="X62">
+        <f t="shared" si="9"/>
+        <v>-8</v>
+      </c>
+      <c r="Y62">
+        <f t="shared" si="9"/>
+        <v>-7</v>
+      </c>
+      <c r="Z62">
+        <f t="shared" si="9"/>
+        <v>-6</v>
+      </c>
+      <c r="AA62">
+        <f t="shared" si="9"/>
+        <v>-5</v>
+      </c>
+      <c r="AB62">
+        <f t="shared" si="9"/>
+        <v>-4</v>
+      </c>
+      <c r="AC62">
+        <f t="shared" si="9"/>
+        <v>-3</v>
+      </c>
+      <c r="AD62">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="9"/>
+        <v>-1</v>
+      </c>
+      <c r="AF62">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>